<commit_message>
update to y axis
</commit_message>
<xml_diff>
--- a/Data/CultureLysoData.xlsx
+++ b/Data/CultureLysoData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://outlookuga-my.sharepoint.com/personal/ccz99536_uga_edu/Documents/Cruises/NES_CCS_Comparison/AcidotropicManuscript/AcidotropicDyes/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="14_{3E5DAE11-4240-B84C-8A20-1DB894A86FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7ABE170D-1F12-044F-B6BE-6A35EFD57BFF}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="14_{3E5DAE11-4240-B84C-8A20-1DB894A86FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD270503-317C-0D4B-867A-792416C992A6}"/>
   <bookViews>
-    <workbookView xWindow="37160" yWindow="-820" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{607BD773-A4C5-F849-B861-90CB68BD1820}"/>
+    <workbookView xWindow="37160" yWindow="-820" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{607BD773-A4C5-F849-B861-90CB68BD1820}"/>
   </bookViews>
   <sheets>
     <sheet name="LysoTracker" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">LysoSensor!$A$1:$H$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LysoTracker!$A$1:$L$72</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3471,7 +3471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86BEE0B4-46AA-5543-A409-0F4EECDF63D9}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
@@ -4645,8 +4645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED9F22E-E12E-E74A-87ED-9CBCE3E6ABE3}">
   <dimension ref="A1:H109"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>